<commit_message>
increase html fig size
</commit_message>
<xml_diff>
--- a/data/contributors.xlsx
+++ b/data/contributors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schilder/Desktop/Ilona_thesis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935D97EA-43AC-DA4B-A330-34508BAF1817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F58830-C2F5-9249-8CC5-FEF76F487F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5960" yWindow="1700" windowWidth="27640" windowHeight="16940" xr2:uid="{3843ECAF-FC15-3B44-AD26-4A902B2E57C4}"/>
+    <workbookView xWindow="1700" yWindow="1020" windowWidth="27640" windowHeight="16940" xr2:uid="{3843ECAF-FC15-3B44-AD26-4A902B2E57C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -621,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8322CDB-25C4-5444-B944-F0725C38DC11}">
   <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91:XFD91"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="75" workbookViewId="0">
+      <selection activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Change graph dims to A0/4
</commit_message>
<xml_diff>
--- a/data/contributors.xlsx
+++ b/data/contributors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schilder/Desktop/Ilona_thesis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C060C57-514A-784A-828F-560762317C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C6BD1A-1C14-B840-9917-8B1C3C5AB764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12120" yWindow="1000" windowWidth="21400" windowHeight="17520" activeTab="1" xr2:uid="{3843ECAF-FC15-3B44-AD26-4A902B2E57C4}"/>
+    <workbookView xWindow="5240" yWindow="1000" windowWidth="28280" windowHeight="17180" activeTab="1" xr2:uid="{3843ECAF-FC15-3B44-AD26-4A902B2E57C4}"/>
   </bookViews>
   <sheets>
     <sheet name="edges" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">edges!$A$1:$C$58</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">nodes!$A$1:$F$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">nodes!$A$1:$F$54</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -661,7 +661,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -689,9 +689,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1316,7 +1313,7 @@
       <c r="A30" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="17" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1324,7 +1321,7 @@
       <c r="A31" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="17" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1852,7 +1849,7 @@
       <c r="A97" t="s">
         <v>43</v>
       </c>
-      <c r="B97" s="21" t="s">
+      <c r="B97" s="20" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1860,7 +1857,7 @@
       <c r="A98" t="s">
         <v>43</v>
       </c>
-      <c r="B98" s="21" t="s">
+      <c r="B98" s="20" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1873,15 +1870,15 @@
       </c>
     </row>
     <row r="100" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A100" s="15" t="s">
+      <c r="A100" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B100" s="15" t="s">
+      <c r="B100" s="14" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A101" s="15" t="s">
+      <c r="A101" s="14" t="s">
         <v>53</v>
       </c>
       <c r="B101" t="s">
@@ -1889,23 +1886,23 @@
       </c>
     </row>
     <row r="102" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A102" s="13" t="s">
+      <c r="A102" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B102" s="13" t="s">
+      <c r="B102" s="12" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A103" s="13" t="s">
+      <c r="A103" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B103" s="13" t="s">
+      <c r="B103" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A104" s="12" t="s">
+      <c r="A104" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B104" t="s">
@@ -1913,7 +1910,7 @@
       </c>
     </row>
     <row r="105" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A105" s="12" t="s">
+      <c r="A105" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B105" t="s">
@@ -1921,7 +1918,7 @@
       </c>
     </row>
     <row r="106" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A106" s="12" t="s">
+      <c r="A106" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B106" s="2" t="s">
@@ -1929,7 +1926,7 @@
       </c>
     </row>
     <row r="107" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A107" s="12" t="s">
+      <c r="A107" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B107" t="s">
@@ -1937,7 +1934,7 @@
       </c>
     </row>
     <row r="108" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A108" s="12" t="s">
+      <c r="A108" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B108" t="s">
@@ -1945,7 +1942,7 @@
       </c>
     </row>
     <row r="109" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A109" s="12" t="s">
+      <c r="A109" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B109" s="2" t="s">
@@ -1953,7 +1950,7 @@
       </c>
     </row>
     <row r="110" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A110" s="12" t="s">
+      <c r="A110" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B110" t="s">
@@ -1961,7 +1958,7 @@
       </c>
     </row>
     <row r="111" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A111" s="12" t="s">
+      <c r="A111" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B111" s="2" t="s">
@@ -1969,7 +1966,7 @@
       </c>
     </row>
     <row r="112" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A112" s="12" t="s">
+      <c r="A112" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B112" s="2" t="s">
@@ -1977,7 +1974,7 @@
       </c>
     </row>
     <row r="113" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A113" s="12" t="s">
+      <c r="A113" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B113" s="2" t="s">
@@ -1985,7 +1982,7 @@
       </c>
     </row>
     <row r="114" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A114" s="12" t="s">
+      <c r="A114" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B114" s="2" t="s">
@@ -1993,7 +1990,7 @@
       </c>
     </row>
     <row r="115" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A115" s="12" t="s">
+      <c r="A115" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B115" s="2" t="s">
@@ -2001,7 +1998,7 @@
       </c>
     </row>
     <row r="116" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A116" s="12" t="s">
+      <c r="A116" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B116" s="2" t="s">
@@ -2018,8 +2015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D721A325-FFE8-414B-B2EB-8286847F0276}">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2138,7 +2135,7 @@
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" ht="68" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -2154,7 +2151,7 @@
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -2170,7 +2167,7 @@
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -2214,7 +2211,7 @@
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="13" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -2230,7 +2227,7 @@
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="13" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -2260,7 +2257,7 @@
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="16" t="s">
         <v>87</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -2276,7 +2273,7 @@
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="16" t="s">
         <v>86</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -2292,7 +2289,7 @@
       <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="16" t="s">
         <v>29</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -2338,7 +2335,7 @@
       <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="14" t="s">
         <v>53</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -2354,7 +2351,7 @@
       <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="14" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -2370,7 +2367,7 @@
       <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="14" t="s">
         <v>31</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -2386,7 +2383,7 @@
       <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="14" t="s">
         <v>52</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -2478,7 +2475,7 @@
       <c r="F29" s="3"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="15" t="s">
         <v>81</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -2492,7 +2489,7 @@
       <c r="F30" s="3"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="18" t="s">
+      <c r="A31" s="17" t="s">
         <v>89</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -2508,7 +2505,7 @@
       <c r="F31" s="3"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -2524,7 +2521,7 @@
       <c r="F32" s="3"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="17" t="s">
         <v>54</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -2540,7 +2537,7 @@
       <c r="F33" s="3"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="17" t="s">
         <v>26</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -2556,7 +2553,7 @@
       <c r="F34" s="3"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="17" t="s">
         <v>104</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -2572,7 +2569,7 @@
       <c r="F35" s="3"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="17" t="s">
         <v>27</v>
       </c>
       <c r="B36" s="3" t="s">
@@ -2588,7 +2585,7 @@
       <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="18" t="s">
+      <c r="A37" s="17" t="s">
         <v>105</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -2604,7 +2601,7 @@
       <c r="F37" s="3"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="18" t="s">
+      <c r="A38" s="17" t="s">
         <v>109</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -2620,7 +2617,7 @@
       <c r="F38" s="3"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="19" t="s">
+      <c r="A39" s="18" t="s">
         <v>21</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -2636,7 +2633,7 @@
       <c r="F39" s="3"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="19" t="s">
+      <c r="A40" s="18" t="s">
         <v>47</v>
       </c>
       <c r="B40" s="3" t="s">
@@ -2652,7 +2649,7 @@
       <c r="F40" s="3"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="18" t="s">
         <v>23</v>
       </c>
       <c r="B41" s="3" t="s">
@@ -2668,7 +2665,7 @@
       <c r="F41" s="3"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="18" t="s">
         <v>24</v>
       </c>
       <c r="B42" s="3" t="s">
@@ -2684,7 +2681,7 @@
       <c r="F42" s="3"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="19" t="s">
+      <c r="A43" s="18" t="s">
         <v>25</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -2700,7 +2697,7 @@
       <c r="F43" s="3"/>
     </row>
     <row r="44" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B44" s="5" t="s">
@@ -2716,14 +2713,14 @@
       <c r="F44" s="3"/>
     </row>
     <row r="45" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A45" s="12" t="s">
-        <v>40</v>
+      <c r="A45" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="D45" s="3">
         <v>20</v>
@@ -2733,16 +2730,14 @@
       </c>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A46" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>119</v>
-      </c>
+    <row r="46" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C46" s="3"/>
       <c r="D46" s="3">
         <v>20</v>
       </c>
@@ -2751,12 +2746,12 @@
       </c>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>34</v>
+        <v>122</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>34</v>
+        <v>122</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3">
@@ -2767,12 +2762,12 @@
       </c>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
-        <v>122</v>
+    <row r="48" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" s="11" t="s">
+        <v>123</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3">
@@ -2783,12 +2778,12 @@
       </c>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
-        <v>123</v>
+    <row r="49" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>123</v>
+        <v>35</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3">
@@ -2799,12 +2794,12 @@
       </c>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
-        <v>35</v>
+    <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A50" s="11" t="s">
+        <v>36</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3">
@@ -2815,12 +2810,12 @@
       </c>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
-        <v>36</v>
+    <row r="51" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3">
@@ -2831,12 +2826,12 @@
       </c>
       <c r="F51" s="3"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>37</v>
+    <row r="52" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A52" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3">
@@ -2847,14 +2842,16 @@
       </c>
       <c r="F52" s="3"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C53" s="3"/>
+    <row r="53" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A53" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>125</v>
+      </c>
       <c r="D53" s="3">
         <v>20</v>
       </c>
@@ -2863,15 +2860,15 @@
       </c>
       <c r="F53" s="3"/>
     </row>
-    <row r="54" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A54" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>125</v>
+    <row r="54" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A54" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="D54" s="3">
         <v>20</v>
@@ -2881,15 +2878,15 @@
       </c>
       <c r="F54" s="3"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>127</v>
+    <row r="55" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A55" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="D55" s="3">
         <v>20</v>
@@ -2900,9 +2897,9 @@
       <c r="F55" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F55" xr:uid="{D721A325-FFE8-414B-B2EB-8286847F0276}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F55">
-      <sortCondition ref="D2:D55"/>
+  <autoFilter ref="A1:F54" xr:uid="{D721A325-FFE8-414B-B2EB-8286847F0276}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F54">
+      <sortCondition ref="D2:D54"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add connections between Sheffield library nodes
</commit_message>
<xml_diff>
--- a/data/contributors.xlsx
+++ b/data/contributors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schilder/Desktop/Ilona_thesis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6096174-8179-6548-B2DB-987EF0AB344D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC98ECD3-6FA2-BA4C-8C1D-7203B7BBDD53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" activeTab="1" xr2:uid="{3843ECAF-FC15-3B44-AD26-4A902B2E57C4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{3843ECAF-FC15-3B44-AD26-4A902B2E57C4}"/>
   </bookViews>
   <sheets>
     <sheet name="edges" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="258">
   <si>
     <t>from</t>
   </si>
@@ -878,7 +878,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="26">
+  <fills count="28">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1029,8 +1029,20 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1077,11 +1089,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1206,6 +1231,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1520,10 +1547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8322CDB-25C4-5444-B944-F0725C38DC11}">
-  <dimension ref="A1:D197"/>
+  <dimension ref="A1:D198"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScale="137" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="137" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3175,6 +3202,14 @@
       </c>
       <c r="D197" s="23"/>
     </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A198" s="52" t="s">
+        <v>140</v>
+      </c>
+      <c r="B198" s="53" t="s">
+        <v>166</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C58" xr:uid="{A8322CDB-25C4-5444-B944-F0725C38DC11}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3185,8 +3220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D721A325-FFE8-414B-B2EB-8286847F0276}">
   <dimension ref="A1:J112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="112" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A92" zoomScale="112" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add more subcluster names
</commit_message>
<xml_diff>
--- a/data/contributors.xlsx
+++ b/data/contributors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schilder/Desktop/Ilona_thesis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC98ECD3-6FA2-BA4C-8C1D-7203B7BBDD53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4451BB-C996-D740-91C6-A12A03B61C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{3843ECAF-FC15-3B44-AD26-4A902B2E57C4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" activeTab="1" xr2:uid="{3843ECAF-FC15-3B44-AD26-4A902B2E57C4}"/>
   </bookViews>
   <sheets>
     <sheet name="edges" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="258">
   <si>
     <t>from</t>
   </si>
@@ -1549,7 +1549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8322CDB-25C4-5444-B944-F0725C38DC11}">
   <dimension ref="A1:D198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="137" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A35" zoomScale="137" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
@@ -3220,8 +3220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D721A325-FFE8-414B-B2EB-8286847F0276}">
   <dimension ref="A1:J112"/>
   <sheetViews>
-    <sheetView topLeftCell="A92" zoomScale="112" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="112" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39:G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3354,7 +3354,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>255</v>
       </c>
@@ -3371,11 +3371,13 @@
       <c r="F6" s="3">
         <v>1</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="5" t="s">
+        <v>255</v>
+      </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>199</v>
       </c>
@@ -3394,11 +3396,13 @@
       <c r="F7" s="3">
         <v>1</v>
       </c>
-      <c r="G7" s="3"/>
+      <c r="G7" s="5" t="s">
+        <v>255</v>
+      </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>11</v>
       </c>
@@ -3417,11 +3421,13 @@
       <c r="F8" s="3">
         <v>1</v>
       </c>
-      <c r="G8" s="3"/>
+      <c r="G8" s="5" t="s">
+        <v>255</v>
+      </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>12</v>
       </c>
@@ -3440,7 +3446,9 @@
       <c r="F9" s="3">
         <v>1</v>
       </c>
-      <c r="G9" s="3"/>
+      <c r="G9" s="5" t="s">
+        <v>255</v>
+      </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
@@ -3461,7 +3469,9 @@
       <c r="F10" s="3">
         <v>2</v>
       </c>
-      <c r="G10" s="3"/>
+      <c r="G10" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
@@ -3482,7 +3492,9 @@
       <c r="F11" s="3">
         <v>2</v>
       </c>
-      <c r="G11" s="3"/>
+      <c r="G11" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
@@ -3505,7 +3517,9 @@
       <c r="F12" s="3">
         <v>2</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
@@ -3528,7 +3542,9 @@
       <c r="F13" s="3">
         <v>2</v>
       </c>
-      <c r="G13" s="3"/>
+      <c r="G13" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
@@ -3549,7 +3565,9 @@
       <c r="F14" s="3">
         <v>3</v>
       </c>
-      <c r="G14" s="3"/>
+      <c r="G14" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
@@ -3572,7 +3590,9 @@
       <c r="F15" s="3">
         <v>3</v>
       </c>
-      <c r="G15" s="3"/>
+      <c r="G15" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
@@ -3595,7 +3615,9 @@
       <c r="F16" s="3">
         <v>3</v>
       </c>
-      <c r="G16" s="3"/>
+      <c r="G16" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
@@ -3618,7 +3640,9 @@
       <c r="F17" s="3">
         <v>3</v>
       </c>
-      <c r="G17" s="3"/>
+      <c r="G17" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
@@ -3639,7 +3663,9 @@
       <c r="F18" s="3">
         <v>4</v>
       </c>
-      <c r="G18" s="3"/>
+      <c r="G18" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
@@ -3662,7 +3688,9 @@
       <c r="F19" s="3">
         <v>4</v>
       </c>
-      <c r="G19" s="3"/>
+      <c r="G19" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
@@ -3685,7 +3713,9 @@
       <c r="F20" s="3">
         <v>4</v>
       </c>
-      <c r="G20" s="3"/>
+      <c r="G20" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
@@ -3708,7 +3738,9 @@
       <c r="F21" s="3">
         <v>4</v>
       </c>
-      <c r="G21" s="3"/>
+      <c r="G21" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
@@ -3731,7 +3763,9 @@
       <c r="F22" s="3">
         <v>4</v>
       </c>
-      <c r="G22" s="3"/>
+      <c r="G22" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
@@ -3754,7 +3788,9 @@
       <c r="F23" s="3">
         <v>4</v>
       </c>
-      <c r="G23" s="3"/>
+      <c r="G23" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
@@ -4128,7 +4164,9 @@
       <c r="F39" s="3">
         <v>8</v>
       </c>
-      <c r="G39" s="3"/>
+      <c r="G39" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
     </row>
@@ -4151,7 +4189,9 @@
       <c r="F40" s="3">
         <v>8</v>
       </c>
-      <c r="G40" s="3"/>
+      <c r="G40" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
     </row>
@@ -4174,7 +4214,9 @@
       <c r="F41" s="3">
         <v>8</v>
       </c>
-      <c r="G41" s="3"/>
+      <c r="G41" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
     </row>
@@ -4197,7 +4239,9 @@
       <c r="F42" s="3">
         <v>8</v>
       </c>
-      <c r="G42" s="3"/>
+      <c r="G42" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
     </row>
@@ -4220,7 +4264,9 @@
       <c r="F43" s="3">
         <v>8</v>
       </c>
-      <c r="G43" s="3"/>
+      <c r="G43" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
     </row>

</xml_diff>

<commit_message>
Add roles back in labels
</commit_message>
<xml_diff>
--- a/data/contributors.xlsx
+++ b/data/contributors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schilder/Desktop/Ilona_thesis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4451BB-C996-D740-91C6-A12A03B61C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A389D5-66B1-4C45-ABE0-0FA6A96538F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" activeTab="1" xr2:uid="{3843ECAF-FC15-3B44-AD26-4A902B2E57C4}"/>
   </bookViews>
@@ -794,9 +794,6 @@
     <t>Manager</t>
   </si>
   <si>
-    <t>Ed Cavanag</t>
-  </si>
-  <si>
     <t>Works Manager</t>
   </si>
   <si>
@@ -848,6 +845,9 @@
   </si>
   <si>
     <t>Archivist, Research Development Specialist, Moving Image &amp; Sound</t>
+  </si>
+  <si>
+    <t>Ed Cavanagh</t>
   </si>
 </sst>
 </file>
@@ -1611,7 +1611,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -1677,7 +1677,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -1693,7 +1693,7 @@
         <v>6</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1866,7 +1866,7 @@
     </row>
     <row r="35" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>200</v>
@@ -1874,7 +1874,7 @@
     </row>
     <row r="36" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>11</v>
@@ -1882,7 +1882,7 @@
     </row>
     <row r="37" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>12</v>
@@ -1890,7 +1890,7 @@
     </row>
     <row r="38" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>13</v>
@@ -1909,7 +1909,7 @@
         <v>13</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="51" x14ac:dyDescent="0.2">
@@ -1925,7 +1925,7 @@
         <v>13</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1933,7 +1933,7 @@
         <v>35</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="51" x14ac:dyDescent="0.2">
@@ -1949,7 +1949,7 @@
         <v>35</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="34" x14ac:dyDescent="0.2">
@@ -2386,7 +2386,7 @@
     </row>
     <row r="100" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B100" t="s">
         <v>3</v>
@@ -2782,7 +2782,7 @@
         <v>154</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
@@ -2843,7 +2843,7 @@
     </row>
     <row r="153" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B153" s="2" t="s">
         <v>34</v>
@@ -2899,7 +2899,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B160" t="s">
         <v>34</v>
@@ -2942,12 +2942,12 @@
         <v>145</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B166" s="2" t="s">
         <v>34</v>
@@ -2982,7 +2982,7 @@
         <v>201</v>
       </c>
       <c r="B170" s="22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3220,8 +3220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D721A325-FFE8-414B-B2EB-8286847F0276}">
   <dimension ref="A1:J112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="112" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39:G43"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="112" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3247,13 +3247,13 @@
         <v>40</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>125</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>39</v>
@@ -3277,7 +3277,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -3299,7 +3299,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -3321,7 +3321,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -3356,10 +3356,10 @@
     </row>
     <row r="6" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="3">
@@ -3372,7 +3372,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -3397,7 +3397,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -3422,7 +3422,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -3447,7 +3447,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -3500,13 +3500,13 @@
     </row>
     <row r="12" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>256</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>257</v>
       </c>
       <c r="D12" s="3">
         <v>1</v>
@@ -3696,7 +3696,7 @@
     </row>
     <row r="20" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>63</v>
@@ -3806,7 +3806,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>242</v>
+        <v>6</v>
       </c>
       <c r="F24" s="3">
         <v>5</v>
@@ -4130,7 +4130,7 @@
         <v>93</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D38" s="3">
         <v>1</v>
@@ -4559,7 +4559,7 @@
         <v>142</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>180</v>
@@ -4579,13 +4579,13 @@
     </row>
     <row r="57" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>247</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>248</v>
       </c>
       <c r="D57" s="3">
         <v>3</v>
@@ -4602,13 +4602,13 @@
     </row>
     <row r="58" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C58" s="5" t="s">
         <v>250</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>251</v>
       </c>
       <c r="D58" s="3">
         <v>3</v>
@@ -5224,7 +5224,7 @@
         <v>6</v>
       </c>
       <c r="G86" s="31" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -5247,15 +5247,15 @@
         <v>6</v>
       </c>
       <c r="G87" s="32" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A88" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B88" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C88" s="30"/>
       <c r="D88" s="3">
@@ -5268,7 +5268,7 @@
         <v>6</v>
       </c>
       <c r="G88" s="31" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -5291,7 +5291,7 @@
         <v>6</v>
       </c>
       <c r="G89" s="31" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -5785,10 +5785,10 @@
         <v>144</v>
       </c>
       <c r="B112" s="33" t="s">
+        <v>257</v>
+      </c>
+      <c r="C112" s="33" t="s">
         <v>240</v>
-      </c>
-      <c r="C112" s="33" t="s">
-        <v>241</v>
       </c>
       <c r="D112" s="3">
         <v>3</v>
@@ -5844,13 +5844,13 @@
         <v>40</v>
       </c>
       <c r="E1" s="50" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F1" s="50" t="s">
         <v>125</v>
       </c>
       <c r="G1" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H1" s="50" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Make self-service part of corr O
</commit_message>
<xml_diff>
--- a/data/contributors.xlsx
+++ b/data/contributors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schilder/Desktop/Ilona_thesis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A389D5-66B1-4C45-ABE0-0FA6A96538F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D672DA2C-4934-B54E-AC41-1FCBA68372FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" activeTab="1" xr2:uid="{3843ECAF-FC15-3B44-AD26-4A902B2E57C4}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="258">
   <si>
     <t>from</t>
   </si>
@@ -3220,8 +3220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D721A325-FFE8-414B-B2EB-8286847F0276}">
   <dimension ref="A1:J112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="112" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="112" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3289,10 +3289,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3">
@@ -3309,38 +3309,37 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="3"/>
+    <row r="4" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="D4" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="F4" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="F4" s="3">
+        <v>10</v>
+      </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="85" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>213</v>
+    </row>
+    <row r="5" spans="1:10" ht="119" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>254</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>60</v>
-      </c>
+        <v>254</v>
+      </c>
+      <c r="C5" s="5"/>
       <c r="D5" s="3">
         <v>1</v>
       </c>
@@ -3348,20 +3347,24 @@
         <v>6</v>
       </c>
       <c r="F5" s="3">
-        <v>10</v>
-      </c>
-      <c r="G5" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>254</v>
+      </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:10" ht="119" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>254</v>
+      <c r="A6" s="12" t="s">
+        <v>199</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="C6" s="5"/>
+        <v>54</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="D6" s="3">
         <v>1</v>
       </c>
@@ -3379,13 +3382,13 @@
     </row>
     <row r="7" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>199</v>
+        <v>11</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>203</v>
+        <v>57</v>
       </c>
       <c r="D7" s="3">
         <v>1</v>
@@ -3404,13 +3407,13 @@
     </row>
     <row r="8" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D8" s="3">
         <v>1</v>
@@ -3427,16 +3430,14 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="119" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>59</v>
-      </c>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="3">
         <v>1</v>
       </c>
@@ -3444,20 +3445,20 @@
         <v>6</v>
       </c>
       <c r="F9" s="3">
-        <v>1</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>254</v>
+        <v>2</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3">
@@ -3475,14 +3476,16 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="3"/>
+    <row r="11" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>256</v>
+      </c>
       <c r="D11" s="3">
         <v>1</v>
       </c>
@@ -3498,15 +3501,15 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>255</v>
+        <v>14</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>255</v>
+        <v>61</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>256</v>
+        <v>62</v>
       </c>
       <c r="D12" s="3">
         <v>1</v>
@@ -3523,16 +3526,14 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>62</v>
-      </c>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="3">
         <v>1</v>
       </c>
@@ -3540,22 +3541,24 @@
         <v>6</v>
       </c>
       <c r="F13" s="3">
-        <v>2</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="3"/>
+    <row r="14" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="D14" s="3">
         <v>1</v>
       </c>
@@ -3573,13 +3576,13 @@
     </row>
     <row r="15" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D15" s="3">
         <v>1</v>
@@ -3598,13 +3601,13 @@
     </row>
     <row r="16" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="D16" s="3">
         <v>1</v>
@@ -3621,16 +3624,14 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>95</v>
-      </c>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="3"/>
       <c r="D17" s="3">
         <v>1</v>
       </c>
@@ -3638,22 +3639,24 @@
         <v>6</v>
       </c>
       <c r="F17" s="3">
-        <v>3</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>22</v>
+        <v>4</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="3"/>
+    <row r="18" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="D18" s="3">
         <v>1</v>
       </c>
@@ -3669,15 +3672,15 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="A19" s="9" t="s">
-        <v>214</v>
+    <row r="19" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="14" t="s">
+        <v>253</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>220</v>
+        <v>63</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="D19" s="3">
         <v>1</v>
@@ -3694,15 +3697,15 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
-        <v>253</v>
+        <v>96</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>64</v>
+        <v>211</v>
       </c>
       <c r="D20" s="3">
         <v>1</v>
@@ -3719,15 +3722,15 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
-        <v>96</v>
+        <v>24</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>211</v>
+        <v>100</v>
       </c>
       <c r="D21" s="3">
         <v>1</v>
@@ -3744,15 +3747,15 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D22" s="3">
         <v>1</v>
@@ -3769,16 +3772,14 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A23" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>99</v>
-      </c>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="3"/>
       <c r="D23" s="3">
         <v>1</v>
       </c>
@@ -3786,20 +3787,23 @@
         <v>6</v>
       </c>
       <c r="F23" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
+      <c r="J23">
+        <v>2</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3">
@@ -3816,18 +3820,17 @@
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
-      <c r="J24">
-        <v>2</v>
-      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="3"/>
+        <v>46</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="D25" s="3">
         <v>1</v>
       </c>
@@ -3845,13 +3848,13 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D26" s="3">
         <v>1</v>
@@ -3870,13 +3873,13 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D27" s="3">
         <v>1</v>
@@ -3895,14 +3898,12 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C28" s="3"/>
       <c r="D28" s="3">
         <v>1</v>
       </c>
@@ -3919,11 +3920,11 @@
       <c r="I28" s="3"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
-        <v>5</v>
+      <c r="A29" s="15" t="s">
+        <v>65</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3">
@@ -3933,22 +3934,22 @@
         <v>6</v>
       </c>
       <c r="F29" s="3">
-        <v>5</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>2</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="15" t="s">
-        <v>65</v>
+      <c r="A30" s="17" t="s">
+        <v>73</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C30" s="3"/>
+        <v>72</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="D30" s="3">
         <v>1</v>
       </c>
@@ -3956,21 +3957,20 @@
         <v>6</v>
       </c>
       <c r="F30" s="3">
-        <v>6</v>
-      </c>
-      <c r="G30" s="3"/>
+        <v>7</v>
+      </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>122</v>
+        <v>75</v>
       </c>
       <c r="D31" s="3">
         <v>1</v>
@@ -3981,18 +3981,19 @@
       <c r="F31" s="3">
         <v>7</v>
       </c>
+      <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D32" s="3">
         <v>1</v>
@@ -4009,13 +4010,13 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D33" s="3">
         <v>1</v>
@@ -4032,13 +4033,13 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D34" s="3">
         <v>1</v>
@@ -4055,13 +4056,13 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D35" s="3">
         <v>1</v>
@@ -4078,13 +4079,13 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D36" s="3">
         <v>1</v>
@@ -4101,13 +4102,13 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>87</v>
+        <v>242</v>
       </c>
       <c r="D37" s="3">
         <v>1</v>
@@ -4123,14 +4124,14 @@
       <c r="I37" s="3"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="17" t="s">
-        <v>93</v>
+      <c r="A38" s="18" t="s">
+        <v>15</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>242</v>
+        <v>79</v>
       </c>
       <c r="D38" s="3">
         <v>1</v>
@@ -4139,18 +4140,20 @@
         <v>6</v>
       </c>
       <c r="F38" s="3">
-        <v>7</v>
-      </c>
-      <c r="G38" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="18" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>79</v>
@@ -4172,10 +4175,10 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="18" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>79</v>
@@ -4197,10 +4200,10 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>79</v>
@@ -4222,10 +4225,10 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>79</v>
@@ -4245,15 +4248,15 @@
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>79</v>
+    <row r="43" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A43" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="D43" s="3">
         <v>1</v>
@@ -4262,35 +4265,35 @@
         <v>6</v>
       </c>
       <c r="F43" s="3">
-        <v>8</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>79</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
     </row>
-    <row r="44" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A44" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>104</v>
-      </c>
+    <row r="44" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="3"/>
       <c r="D44" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F44" s="3">
-        <v>9</v>
-      </c>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H44" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="I44" s="3"/>
     </row>
     <row r="45" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4305,12 +4308,14 @@
         <v>2</v>
       </c>
       <c r="E45" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F45" s="3">
+        <v>1</v>
+      </c>
+      <c r="G45" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F45" s="3">
-        <v>1</v>
-      </c>
-      <c r="G45" s="3"/>
       <c r="H45" s="3" t="b">
         <v>1</v>
       </c>
@@ -4328,12 +4333,14 @@
         <v>2</v>
       </c>
       <c r="E46" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F46" s="3">
+        <v>1</v>
+      </c>
+      <c r="G46" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F46" s="3">
-        <v>1</v>
-      </c>
-      <c r="G46" s="3"/>
       <c r="H46" s="3" t="b">
         <v>1</v>
       </c>
@@ -4351,12 +4358,14 @@
         <v>2</v>
       </c>
       <c r="E47" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F47" s="3">
+        <v>1</v>
+      </c>
+      <c r="G47" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F47" s="3">
-        <v>1</v>
-      </c>
-      <c r="G47" s="3"/>
       <c r="H47" s="3" t="b">
         <v>1</v>
       </c>
@@ -4376,12 +4385,14 @@
         <v>2</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F48" s="3">
         <v>2</v>
       </c>
-      <c r="G48" s="3"/>
+      <c r="G48" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="H48" s="3" t="b">
         <v>1</v>
       </c>
@@ -4399,12 +4410,14 @@
         <v>2</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F49" s="3">
         <v>2</v>
       </c>
-      <c r="G49" s="3"/>
+      <c r="G49" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="H49" s="3" t="b">
         <v>1</v>
       </c>
@@ -4422,12 +4435,14 @@
         <v>2</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F50" s="3">
         <v>2</v>
       </c>
-      <c r="G50" s="3"/>
+      <c r="G50" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="H50" s="3" t="b">
         <v>1</v>
       </c>
@@ -4445,12 +4460,14 @@
         <v>2</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F51" s="3">
         <v>2</v>
       </c>
-      <c r="G51" s="3"/>
+      <c r="G51" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="H51" s="3" t="b">
         <v>1</v>
       </c>
@@ -4468,12 +4485,14 @@
         <v>2</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F52" s="3">
         <v>2</v>
       </c>
-      <c r="G52" s="3"/>
+      <c r="G52" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="H52" s="3" t="b">
         <v>1</v>
       </c>
@@ -4493,12 +4512,14 @@
         <v>2</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F53" s="3">
         <v>2</v>
       </c>
-      <c r="G53" s="3"/>
+      <c r="G53" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="H53" s="3" t="b">
         <v>1</v>
       </c>
@@ -4518,12 +4539,14 @@
         <v>2</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F54" s="3">
         <v>2</v>
       </c>
-      <c r="G54" s="3"/>
+      <c r="G54" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="H54" s="3" t="b">
         <v>1</v>
       </c>
@@ -4543,12 +4566,14 @@
         <v>2</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F55" s="3">
         <v>2</v>
       </c>
-      <c r="G55" s="3"/>
+      <c r="G55" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="H55" s="3" t="b">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Make self-service part of corr O 2
</commit_message>
<xml_diff>
--- a/data/contributors.xlsx
+++ b/data/contributors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schilder/Desktop/Ilona_thesis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D672DA2C-4934-B54E-AC41-1FCBA68372FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37302756-6DD3-C742-8173-F723D60486E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" activeTab="1" xr2:uid="{3843ECAF-FC15-3B44-AD26-4A902B2E57C4}"/>
   </bookViews>
@@ -3220,8 +3220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D721A325-FFE8-414B-B2EB-8286847F0276}">
   <dimension ref="A1:J112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="112" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="112" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>